<commit_message>
cucumber dry run test cases exectued successfully
</commit_message>
<xml_diff>
--- a/selenium-quick-start/src/test/resources/test-data/test-data-file.xlsx
+++ b/selenium-quick-start/src/test/resources/test-data/test-data-file.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="login-data" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,12 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t xml:space="preserve">Username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password</t>
+  </si>
   <si>
     <t xml:space="preserve">test1@test.com</t>
   </si>
   <si>
     <t xml:space="preserve">password1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test2@test.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password2</t>
   </si>
 </sst>
 </file>
@@ -35,7 +47,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -64,13 +76,26 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -107,12 +132,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -239,28 +284,45 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.09"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="test1@test.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="test1@test.com"/>
+    <hyperlink ref="A3" r:id="rId2" display="test2@test.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>